<commit_message>
HTML e formatação do email
</commit_message>
<xml_diff>
--- a/files/PlanilhaFuturosFuncionarios.xlsx
+++ b/files/PlanilhaFuturosFuncionarios.xlsx
@@ -1,91 +1,64 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EmailBot\files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-75" windowWidth="20730" windowHeight="11160"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-18540" yWindow="1995" windowWidth="15375" windowHeight="7875" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Matheus Diniz</t>
-  </si>
-  <si>
-    <t>matheusinhodinizinho@gmail.com</t>
-  </si>
-  <si>
-    <t>ENVIADO</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -105,30 +78,89 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -394,77 +426,117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col width="30.7109375" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="32.140625" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3" s="3"/>
-      <c r="C3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4" s="3"/>
-      <c r="C4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="4"/>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Matheus Diniz</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>matheusinhodinizinho@gmail.com</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ENVIADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Dóris Andressa Moura Luvizute</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>doriluvizute@gmail.com</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Email inválido</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bruno  da Silva</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>dorisluvizute@gmail.com</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ENVIADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n"/>
+      <c r="B5" s="5" t="n"/>
+      <c r="C5" s="4" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n"/>
+      <c r="B6" s="6" t="n"/>
+      <c r="C6" s="4" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n"/>
+      <c r="B7" s="6" t="n"/>
+      <c r="C7" s="4" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n"/>
+      <c r="B8" s="6" t="n"/>
+      <c r="C8" s="4" t="n"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IMAP e SMTP coporativo
</commit_message>
<xml_diff>
--- a/files/PlanilhaFuturosFuncionarios.xlsx
+++ b/files/PlanilhaFuturosFuncionarios.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-18540" yWindow="1995" windowWidth="15375" windowHeight="7875" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7875" windowWidth="15375" xWindow="-18540" yWindow="1995"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
@@ -74,25 +74,25 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="8" name="Hiperlink" xfId="1"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -439,9 +439,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="30.7109375" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="32.140625" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="13.5703125" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="2" width="30.7109375"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="2" width="32.140625"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="2" width="13.5703125"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -498,17 +498,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bruno  da Silva</t>
+          <t>Dóris Andressa Moura Luvizute</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
           <t>dorisluvizute@gmail.com</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ENVIADO</t>
         </is>
       </c>
     </row>
@@ -536,7 +531,7 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageMargins bottom="0.787401575" footer="0.31496062" header="0.31496062" left="0.511811024" right="0.511811024" top="0.787401575"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
criação de dois bots para envio e verificação
</commit_message>
<xml_diff>
--- a/files/PlanilhaFuturosFuncionarios.xlsx
+++ b/files/PlanilhaFuturosFuncionarios.xlsx
@@ -431,10 +431,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="A4:B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -464,12 +464,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Matheus Diniz</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>matheusinhodinizinho@gmail.com</t>
+          <t>Dóris Andressa Moura Luvizute</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>dorisluvizute@gmail.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -477,6 +477,7 @@
           <t>ENVIADO</t>
         </is>
       </c>
+      <c r="E2" s="4" t="n"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -484,33 +485,19 @@
           <t>Dóris Andressa Moura Luvizute</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="6" t="inlineStr">
         <is>
           <t>doriluvizute@gmail.com</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="4" t="inlineStr">
         <is>
           <t>Email inválido</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Dóris Andressa Moura Luvizute</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>dorisluvizute@gmail.com</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ENVIADO</t>
-        </is>
-      </c>
+      <c r="B4" s="3" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="n"/>
@@ -534,7 +521,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins bottom="0.787401575" footer="0.31496062" header="0.31496062" left="0.511811024" right="0.511811024" top="0.787401575"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
Alterações feitas para prod
</commit_message>
<xml_diff>
--- a/files/PlanilhaFuturosFuncionarios.xlsx
+++ b/files/PlanilhaFuturosFuncionarios.xlsx
@@ -80,12 +80,12 @@
   <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -434,14 +434,14 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="2" width="30.7109375"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="2" width="32.140625"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="2" width="13.5703125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="5" width="35.28515625"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="5" width="32.140625"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="5" width="13.5703125"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -464,12 +464,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Dóris Andressa Moura Luvizute</t>
+          <t>Gleyse Oliveira Rosal</t>
         </is>
       </c>
       <c r="B2" s="6" t="inlineStr">
         <is>
-          <t>dorisluvizute@gmail.com</t>
+          <t>gleyseor@gmail.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -477,52 +477,38 @@
           <t>ENVIADO</t>
         </is>
       </c>
-      <c r="E2" s="4" t="n"/>
+      <c r="E2" s="3" t="n"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dóris Andressa Moura Luvizute</t>
-        </is>
-      </c>
-      <c r="B3" s="6" t="inlineStr">
-        <is>
-          <t>doriluvizute@gmail.com</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>Email inválido</t>
+          <t>Erasmo Rosa Dos Reis</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>erasmo.reis@bol.com.br</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ENVIADO</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="3" t="n"/>
+      <c r="B4" s="4" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="n"/>
-      <c r="B5" s="5" t="n"/>
-      <c r="C5" s="4" t="n"/>
+      <c r="B5" s="2" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="n"/>
-      <c r="B6" s="6" t="n"/>
-      <c r="C6" s="4" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="n"/>
-      <c r="B7" s="6" t="n"/>
-      <c r="C7" s="4" t="n"/>
+      <c r="B6" s="2" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="n"/>
-      <c r="B8" s="6" t="n"/>
-      <c r="C8" s="4" t="n"/>
+      <c r="B8" s="2" t="n"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins bottom="0.787401575" footer="0.31496062" header="0.31496062" left="0.511811024" right="0.511811024" top="0.787401575"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>

</xml_diff>